<commit_message>
Add missing 4BLD for Peter Andersson
</commit_message>
<xml_diff>
--- a/data/2021-11-29/SCW Weekly Comp 2021-11-29 (Responses).xlsx
+++ b/data/2021-11-29/SCW Weekly Comp 2021-11-29 (Responses).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="209">
   <si>
     <t>Timestamp</t>
   </si>
@@ -632,6 +632,12 @@
   </si>
   <si>
     <t>1:03.95</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/413306813768770?post_id=418041409961977&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>11:38.97</t>
   </si>
 </sst>
 </file>
@@ -3201,6 +3207,41 @@
         <v>57.29</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" s="2">
+        <v>44543.61594304398</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="CT52" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="CU52" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="CV52" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="CW52" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="CX52" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="F2"/>
@@ -3253,7 +3294,8 @@
     <hyperlink r:id="rId48" ref="F49"/>
     <hyperlink r:id="rId49" ref="F50"/>
     <hyperlink r:id="rId50" ref="F51"/>
+    <hyperlink r:id="rId51" ref="F52"/>
   </hyperlinks>
-  <drawing r:id="rId51"/>
+  <drawing r:id="rId52"/>
 </worksheet>
 </file>
</xml_diff>